<commit_message>
Implemented name comparison which ignores titles
</commit_message>
<xml_diff>
--- a/docs/addresses to process.xlsx
+++ b/docs/addresses to process.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\Desktop\FlatFinder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D629222-76EB-4E77-A210-975EEE8BC8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987188B8-FE71-44D3-8DA6-C0E0B54701E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C52F1565-2249-48A7-8512-6E05E9D60EC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C52F1565-2249-48A7-8512-6E05E9D60EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -881,10 +881,13 @@
   <dimension ref="A1:X80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1459,6 +1462,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>